<commit_message>
added one strategy to the list
</commit_message>
<xml_diff>
--- a/Strategies.xlsx
+++ b/Strategies.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6" uniqueCount="6">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="11" uniqueCount="10">
   <si>
     <t>ID</t>
   </si>
@@ -37,6 +37,18 @@
   </si>
   <si>
     <t>Market_Ineficiency</t>
+  </si>
+  <si>
+    <t>FALCON_A</t>
+  </si>
+  <si>
+    <t>Trade Eucledian kNN. Entry using cross_macd and calculated probabilities to enter using kNN machine learning</t>
+  </si>
+  <si>
+    <t>When MACD indicator changing direction</t>
+  </si>
+  <si>
+    <t>Ranging market</t>
   </si>
 </sst>
 </file>
@@ -72,8 +84,11 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -354,10 +369,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:F1"/>
+  <dimension ref="A1:F2"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C11" sqref="C11"/>
+      <selection activeCell="F2" sqref="F2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -390,6 +405,26 @@
         <v>5</v>
       </c>
     </row>
+    <row r="2" spans="1:6" ht="60" x14ac:dyDescent="0.25">
+      <c r="A2">
+        <v>33</v>
+      </c>
+      <c r="B2" t="s">
+        <v>6</v>
+      </c>
+      <c r="C2" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="D2" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="E2" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="F2" s="1" t="s">
+        <v>9</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
added sheet 2 to write log of our thoughts
</commit_message>
<xml_diff>
--- a/Strategies.xlsx
+++ b/Strategies.xlsx
@@ -4,10 +4,11 @@
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="18730"/>
   <workbookPr filterPrivacy="1"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="162913"/>
   <extLst>
@@ -19,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="21" uniqueCount="18">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="24" uniqueCount="20">
   <si>
     <t>ID</t>
   </si>
@@ -73,6 +74,12 @@
   </si>
   <si>
     <t>Moving Average cross over system. Aided by AI guess on Market Status</t>
+  </si>
+  <si>
+    <t>Date</t>
+  </si>
+  <si>
+    <t>Log</t>
   </si>
 </sst>
 </file>
@@ -395,7 +402,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:F4"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="C8" sqref="C8"/>
     </sheetView>
   </sheetViews>
@@ -492,4 +499,33 @@
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:C1"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A2" sqref="A2"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="3" max="3" width="104.7109375" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" t="s">
+        <v>18</v>
+      </c>
+      <c r="C1" t="s">
+        <v>19</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
added filter for strategy
</commit_message>
<xml_diff>
--- a/Strategies.xlsx
+++ b/Strategies.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="18730"/>
   <workbookPr filterPrivacy="1"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645" activeTab="1"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="24" uniqueCount="20">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="28" uniqueCount="24">
   <si>
     <t>ID</t>
   </si>
@@ -80,6 +80,20 @@
   </si>
   <si>
     <t>Log</t>
+  </si>
+  <si>
+    <t>FALCON_R</t>
+  </si>
+  <si>
+    <t>Capturing reverting ranging markets</t>
+  </si>
+  <si>
+    <t>Sell: SuperSmoother crosses Keltner Channels from Top;
+Buy: SupSmooth crosses Keltner Channels from Bottom</t>
+  </si>
+  <si>
+    <t>Price goes against Keltner channel with bigger multiplier;
+Price hit take profit which is either: 3x more than stop loss or we go and cross opposite side of the channel</t>
   </si>
 </sst>
 </file>
@@ -400,10 +414,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:F4"/>
+  <dimension ref="A1:F5"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C8" sqref="C8"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E6" sqref="E6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -496,6 +510,23 @@
         <v>12</v>
       </c>
     </row>
+    <row r="5" spans="1:6" ht="90" x14ac:dyDescent="0.25">
+      <c r="A5">
+        <v>35</v>
+      </c>
+      <c r="B5" t="s">
+        <v>20</v>
+      </c>
+      <c r="C5" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="D5" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="E5" s="1" t="s">
+        <v>23</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -505,7 +536,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:C1"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
updated with new strategy
</commit_message>
<xml_diff>
--- a/Strategies.xlsx
+++ b/Strategies.xlsx
@@ -1,7 +1,7 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="18730"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="19029"/>
   <workbookPr filterPrivacy="1"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12795"/>
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="25" uniqueCount="22">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="30" uniqueCount="27">
   <si>
     <t>ID</t>
   </si>
@@ -87,6 +87,21 @@
   <si>
     <t>Price goes against Keltner channel with bigger multiplier;
 Price hit take profit which is either: 3x more than stop loss or we go and cross opposite side of the channel</t>
+  </si>
+  <si>
+    <t>FALCON_S</t>
+  </si>
+  <si>
+    <t>Trade according to news sentiment</t>
+  </si>
+  <si>
+    <t>8hours - time based</t>
+  </si>
+  <si>
+    <t>Assumed that politicians or media are creating impulses that leading the market</t>
+  </si>
+  <si>
+    <t>Sentiment Polarity Score is calculated from countries news for Base and quoted currencies. Entry if too big difference between sentiment scores.</t>
   </si>
 </sst>
 </file>
@@ -407,10 +422,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:F5"/>
+  <dimension ref="A1:F6"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E11" sqref="E11"/>
+      <selection activeCell="D7" sqref="D7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -520,6 +535,26 @@
         <v>21</v>
       </c>
     </row>
+    <row r="6" spans="1:6" ht="90" x14ac:dyDescent="0.25">
+      <c r="A6">
+        <v>36</v>
+      </c>
+      <c r="B6" t="s">
+        <v>22</v>
+      </c>
+      <c r="C6" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="D6" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="E6" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="F6" s="1" t="s">
+        <v>25</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
have the file name matching the data log
</commit_message>
<xml_diff>
--- a/Strategies.xlsx
+++ b/Strategies.xlsx
@@ -1,9 +1,9 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="19330"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="20325"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:8100000_{14763621-282B-4C31-9E12-BC43C06749A7}" xr6:coauthVersionLast="33" xr6:coauthVersionMax="33" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:8100000_{D746831F-51EE-462D-8D98-AF81DD1C2D98}" xr6:coauthVersionLast="34" xr6:coauthVersionMax="34" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12795" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="40" uniqueCount="33">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="45" uniqueCount="35">
   <si>
     <t>ID</t>
   </si>
@@ -121,6 +121,12 @@
   </si>
   <si>
     <t>when prediction time has expired or targets were reached</t>
+  </si>
+  <si>
+    <t>FALCON_F2</t>
+  </si>
+  <si>
+    <t>Trade Entry and Treshold is predicted from AI</t>
   </si>
 </sst>
 </file>
@@ -441,10 +447,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:F8"/>
+  <dimension ref="A1:F9"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C8" sqref="C8"/>
+      <selection activeCell="D9" sqref="D9:F9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -614,6 +620,26 @@
         <v>31</v>
       </c>
     </row>
+    <row r="9" spans="1:6" ht="45" x14ac:dyDescent="0.25">
+      <c r="A9">
+        <v>39</v>
+      </c>
+      <c r="B9" t="s">
+        <v>33</v>
+      </c>
+      <c r="C9" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="D9" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="E9" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="F9" s="1" t="s">
+        <v>31</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
changed the file name to read prices values
</commit_message>
<xml_diff>
--- a/Strategies.xlsx
+++ b/Strategies.xlsx
@@ -1,9 +1,9 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="20325"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="21001"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:8100000_{D746831F-51EE-462D-8D98-AF81DD1C2D98}" xr6:coauthVersionLast="34" xr6:coauthVersionMax="34" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{41B5BBEA-AD80-43F2-B864-EC15E2F34F96}" xr6:coauthVersionLast="38" xr6:coauthVersionMax="38" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12795" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -450,7 +450,7 @@
   <dimension ref="A1:F9"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D9" sqref="D9:F9"/>
+      <selection activeCell="A3" sqref="A3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -485,7 +485,7 @@
     </row>
     <row r="2" spans="1:6" ht="60" x14ac:dyDescent="0.25">
       <c r="A2">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="B2" t="s">
         <v>6</v>

</xml_diff>